<commit_message>
Modification de la dernière version pour pouvoir choisir entre fichier grib et fichier excel pour le vent
</commit_message>
<xml_diff>
--- a/Logiciel/Données_vent/Vent.xlsx
+++ b/Logiciel/Données_vent/Vent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/847b627be5f97550/Arthur/Programmation/TIPE_Arthur_Lhoste/Logiciel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/847b627be5f97550/Arthur/Programmation/Projet_routage/TIPE_Arthur_Lhoste/Logiciel/Données_vent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="362" documentId="8_{6AB1F8BF-0BCE-45DB-A9FF-250C9FC49FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE6C15CF-AC02-413E-829A-FAC6217F81B3}"/>
+  <xr:revisionPtr revIDLastSave="369" documentId="8_{6AB1F8BF-0BCE-45DB-A9FF-250C9FC49FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDA9D100-60E3-4896-B26C-563D848F05D5}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{A973CA7D-4A48-4D4D-AB61-1755BF5454FC}"/>
+    <workbookView xWindow="34452" yWindow="2940" windowWidth="30936" windowHeight="16776" xr2:uid="{A973CA7D-4A48-4D4D-AB61-1755BF5454FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
     <t>5;5</t>
   </si>
   <si>
-    <t>0;20</t>
+    <t>-5;-5</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
   <dimension ref="A1:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -497,7 +497,7 @@
         <v>3.2</v>
       </c>
       <c r="C2">
-        <v>0.05</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -511,44 +511,43 @@
         <v>7</v>
       </c>
       <c r="B4" s="1">
-        <f>B2</f>
-        <v>3.2</v>
+        <v>-9</v>
       </c>
       <c r="C4" s="1">
         <f>B4+$C$2</f>
-        <v>3.25</v>
+        <v>-8</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" ref="D4:I4" si="0">C4+$C$2</f>
-        <v>3.3</v>
+        <v>-7</v>
       </c>
       <c r="E4" s="1">
         <f t="shared" si="0"/>
-        <v>3.3499999999999996</v>
+        <v>-6</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>3.3999999999999995</v>
+        <v>-5</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="0"/>
-        <v>3.4499999999999993</v>
+        <v>-4</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="0"/>
-        <v>3.4999999999999991</v>
+        <v>-3</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>3.5499999999999989</v>
+        <v>-2</v>
       </c>
       <c r="J4" s="1">
         <f t="shared" ref="J4" si="1">I4+$C$2</f>
-        <v>3.5999999999999988</v>
+        <v>-1</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" ref="K4" si="2">J4+$C$2</f>
-        <v>3.6499999999999986</v>
+        <v>0</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -559,8 +558,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
-        <f>A2</f>
-        <v>47.7</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -572,10 +570,10 @@
         <v>8</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>9</v>
@@ -602,7 +600,7 @@
     <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <f>A5-$C$2</f>
-        <v>47.650000000000006</v>
+        <v>47</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -614,10 +612,10 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>9</v>
@@ -644,7 +642,7 @@
     <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <f t="shared" ref="A7:A10" si="3">A6-$C$2</f>
-        <v>47.600000000000009</v>
+        <v>46</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -656,10 +654,10 @@
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>9</v>
@@ -686,7 +684,7 @@
     <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <f t="shared" si="3"/>
-        <v>47.550000000000011</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -698,10 +696,10 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>9</v>
@@ -728,7 +726,7 @@
     <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <f t="shared" si="3"/>
-        <v>47.500000000000014</v>
+        <v>44</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -740,10 +738,10 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>9</v>
@@ -770,7 +768,7 @@
     <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <f t="shared" si="3"/>
-        <v>47.450000000000017</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -782,10 +780,10 @@
         <v>8</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>9</v>
@@ -812,7 +810,7 @@
     <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <f>A10-$C$2</f>
-        <v>47.40000000000002</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -824,10 +822,10 @@
         <v>8</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>9</v>

</xml_diff>